<commit_message>
graphics update and preliminar regression
</commit_message>
<xml_diff>
--- a/Horas.xlsx
+++ b/Horas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b2b7969831da8e18/Documentos/RA_JPV_JIG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{2BA29DE2-20B8-4E89-9115-24A9D1E7063F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7FBFC45E-4034-4A9C-928D-4DC395FF2E50}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{2BA29DE2-20B8-4E89-9115-24A9D1E7063F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CB3C2528-B5DD-450A-8A98-809D8C8A4664}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Figure of share of sales: initial proposal</t>
+  </si>
+  <si>
+    <t>Figure of share of sales: new graphics and variables</t>
   </si>
 </sst>
 </file>
@@ -320,10 +323,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -398,6 +401,17 @@
         <v>9</v>
       </c>
     </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>43971</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
productive linkages initial proposal: histograms and scatter plots
</commit_message>
<xml_diff>
--- a/Horas.xlsx
+++ b/Horas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b2b7969831da8e18/Documentos/RA_JPV_JIG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{2BA29DE2-20B8-4E89-9115-24A9D1E7063F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7EAD4D81-D466-4585-BE1E-76D218FD750D}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{2BA29DE2-20B8-4E89-9115-24A9D1E7063F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CD6617DF-D5E4-4519-974B-C60AF29E2E9E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -62,6 +62,15 @@
   </si>
   <si>
     <t>05/21/2020</t>
+  </si>
+  <si>
+    <t>05/31/2020</t>
+  </si>
+  <si>
+    <t>Figures: productive linkages task 3.1 (complete) and 3.2 (in progress)</t>
+  </si>
+  <si>
+    <t>Figures: productive linkages part 3.1 and 3.2 initial proposal</t>
   </si>
 </sst>
 </file>
@@ -333,10 +342,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -433,6 +442,28 @@
         <v>12</v>
       </c>
     </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>43836</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changing the base for creation rates
</commit_message>
<xml_diff>
--- a/Horas.xlsx
+++ b/Horas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b2b7969831da8e18/Documentos/RA_JPV_JIG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{2BA29DE2-20B8-4E89-9115-24A9D1E7063F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CD6617DF-D5E4-4519-974B-C60AF29E2E9E}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{2BA29DE2-20B8-4E89-9115-24A9D1E7063F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4A513E20-E87E-4DAD-8C3F-985A53BF2736}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -37,49 +37,37 @@
     <t>Corrections and final tool</t>
   </si>
   <si>
-    <t>05/13/2020-05/18/2020</t>
-  </si>
-  <si>
     <t>Corrections and optimization of the distances code</t>
   </si>
   <si>
     <t>Trade: inter-regions distance calculations initial proposal</t>
   </si>
   <si>
-    <t>05/19/2020</t>
-  </si>
-  <si>
     <t>Figure of share of sales: initial proposal</t>
   </si>
   <si>
     <t>Figure of share of sales: new graphics and variables</t>
   </si>
   <si>
-    <t>05/20/2020</t>
-  </si>
-  <si>
     <t>Figure of share of sales: corrections, regressions and pending graphics</t>
   </si>
   <si>
-    <t>05/21/2020</t>
-  </si>
-  <si>
-    <t>05/31/2020</t>
-  </si>
-  <si>
-    <t>Figures: productive linkages task 3.1 (complete) and 3.2 (in progress)</t>
-  </si>
-  <si>
-    <t>Figures: productive linkages part 3.1 and 3.2 initial proposal</t>
+    <t>Figure of share of sales: productive linkages task 3.1 (complete) and 3.2 (in progress)</t>
+  </si>
+  <si>
+    <t>Figure of share of sales: productive linkages part 3.1 and 3.2 initial proposal</t>
+  </si>
+  <si>
+    <t>Figure of share of sales: Task 3.3., survival and creation rates plots initial proposal</t>
+  </si>
+  <si>
+    <t>Algorithm design for task 3.4.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -116,14 +104,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -342,16 +328,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B2" sqref="B2:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
@@ -366,8 +352,8 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
-        <v>43835</v>
+      <c r="A2" s="4">
+        <v>43952</v>
       </c>
       <c r="B2" s="1">
         <v>2</v>
@@ -377,8 +363,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
-        <v>43866</v>
+      <c r="A3" s="4">
+        <v>43953</v>
       </c>
       <c r="B3" s="1">
         <v>0.5</v>
@@ -389,79 +375,101 @@
     </row>
     <row r="4" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
-        <v>44170</v>
+        <v>43963</v>
       </c>
       <c r="B4" s="2">
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
+      <c r="A5" s="3">
+        <v>43969</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>8</v>
+      <c r="A6" s="3">
+        <v>43970</v>
       </c>
       <c r="B6">
         <v>1.5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>11</v>
+      <c r="A7" s="3">
+        <v>43971</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>13</v>
+      <c r="A8" s="3">
+        <v>43972</v>
       </c>
       <c r="B8">
         <v>3.5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>14</v>
+      <c r="A9" s="3">
+        <v>43982</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
-        <v>43836</v>
+      <c r="A10" s="3">
+        <v>43983</v>
       </c>
       <c r="B10">
         <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>43986</v>
+      </c>
+      <c r="B11">
+        <v>1.25</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>43987</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
survival function estimation and plotting: initial proposal
</commit_message>
<xml_diff>
--- a/Horas.xlsx
+++ b/Horas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b2b7969831da8e18/Documentos/RA_JPV_JIG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{2BA29DE2-20B8-4E89-9115-24A9D1E7063F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4A513E20-E87E-4DAD-8C3F-985A53BF2736}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{2BA29DE2-20B8-4E89-9115-24A9D1E7063F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F0A539C4-A055-4E96-BB39-63577E551F29}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>Algorithm design for task 3.4.</t>
+  </si>
+  <si>
+    <t>Figure of share of sales: Task 3.4 survival function estimation and plotting, initial proposal</t>
   </si>
 </sst>
 </file>
@@ -328,16 +331,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="76.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
@@ -472,6 +475,17 @@
         <v>13</v>
       </c>
     </row>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>43988</v>
+      </c>
+      <c r="B13">
+        <v>2.5</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
weighted survival function and checking variables
</commit_message>
<xml_diff>
--- a/Horas.xlsx
+++ b/Horas.xlsx
@@ -1,25 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose Pablo\Dropbox\0-mycomputer\mydocuments\0-LSE\0-Reseach\Z-RAs\RA_JPV_JIG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b2b7969831da8e18/Documentos/RA_JPV_JIG/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="5" documentId="114_{EC8BD569-CF25-46ED-8EBE-08CA7A09F399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{24FBF07F-44BB-4371-B73D-8846D9761617}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -70,12 +81,15 @@
   </si>
   <si>
     <t>Hours pending to be paid:</t>
+  </si>
+  <si>
+    <t>Figure of share of sales: task 3.4 options for weighted survival function and checking S(1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -349,32 +363,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="76.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="76.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B1">
         <f>+SUM(B4:B1048576)</f>
-        <v>-2.75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="12.45" x14ac:dyDescent="0.3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -385,7 +399,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>43952</v>
       </c>
@@ -396,7 +410,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>43953</v>
       </c>
@@ -407,7 +421,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>43963</v>
       </c>
@@ -418,7 +432,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>43969</v>
       </c>
@@ -429,7 +443,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>43970</v>
       </c>
@@ -440,7 +454,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>43971</v>
       </c>
@@ -451,7 +465,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>43972</v>
       </c>
@@ -462,7 +476,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>43982</v>
       </c>
@@ -473,7 +487,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>43983</v>
       </c>
@@ -484,7 +498,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>43986</v>
       </c>
@@ -495,7 +509,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>43987</v>
       </c>
@@ -506,7 +520,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>43988</v>
       </c>
@@ -517,7 +531,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>43989</v>
       </c>
@@ -526,6 +540,17 @@
       </c>
       <c r="C16" s="6" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>43991</v>
+      </c>
+      <c r="B17">
+        <v>1.75</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Initial commit of Matching ORBIS and DENUE
</commit_message>
<xml_diff>
--- a/Horas.xlsx
+++ b/Horas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b2b7969831da8e18/Documentos/RA_JPV_JIG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="143" documentId="114_{EC8BD569-CF25-46ED-8EBE-08CA7A09F399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CB595AF6-71E7-4601-9D3A-A1C7A714DF5A}"/>
+  <xr:revisionPtr revIDLastSave="164" documentId="114_{EC8BD569-CF25-46ED-8EBE-08CA7A09F399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C5493D06-B372-4DE2-BA26-8C598A726680}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -135,6 +135,18 @@
   </si>
   <si>
     <t>Coding RapidFuzz algorithm and scaling</t>
+  </si>
+  <si>
+    <t>Data set corrections</t>
+  </si>
+  <si>
+    <t>RapidFuzz parallel programming</t>
+  </si>
+  <si>
+    <t>RapidFuzz parallel programming and final matches data set</t>
+  </si>
+  <si>
+    <t>Documentation</t>
   </si>
 </sst>
 </file>
@@ -419,10 +431,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -439,7 +451,7 @@
       </c>
       <c r="B1" s="1">
         <f>+SUM(B4:B1048576)</f>
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -880,6 +892,61 @@
       </c>
       <c r="C42" s="2" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="5">
+        <v>44093</v>
+      </c>
+      <c r="B43" s="1">
+        <v>1</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="5">
+        <v>44094</v>
+      </c>
+      <c r="B44" s="1">
+        <v>1</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="5">
+        <v>44095</v>
+      </c>
+      <c r="B45" s="1">
+        <v>2</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="5">
+        <v>44097</v>
+      </c>
+      <c r="B46" s="1">
+        <v>1</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="5">
+        <v>44098</v>
+      </c>
+      <c r="B47" s="1">
+        <v>1</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>